<commit_message>
# This is a combination of 11 commits. # This is the 1st commit message:
end to end workflow test

# This is the commit message #2:

removed extraneous file

# This is the commit message #3:

added number of participants

# This is the commit message #4:

debugging travis

# This is the commit message #5:

changed value of cells in sample file

# This is the commit message #6:

checking for number of submissions in history

# This is the commit message #7:

debugging travis

# This is the commit message #8:

extended time for data submission

# This is the commit message #9:

changed sample file

# This is the commit message #10:

added identifier to the submission success modal

# This is the commit message #11:

changed mechanism for checking successful submission
</commit_message>
<xml_diff>
--- a/test/selenium/files/bwwc.xlsx
+++ b/test/selenium/files/bwwc.xlsx
@@ -5,11 +5,11 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lucyqin/Documents/multiparty/web-mpc/test/cafe/files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lucyqin/Documents/multiparty/web-mpc/test/selenium/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16520" activeTab="2"/>
+    <workbookView xWindow="6280" yWindow="1000" windowWidth="28800" windowHeight="16520" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Enter Data →" sheetId="19" r:id="rId1"/>
@@ -631,7 +631,127 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="23">
+  <dxfs count="35">
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -1158,8 +1278,8 @@
   </sheetPr>
   <dimension ref="A1:Z18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S14" sqref="S14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1950,7 +2070,7 @@
     <mergeCell ref="J5:K5"/>
   </mergeCells>
   <conditionalFormatting sqref="B7:Q16">
-    <cfRule type="cellIs" dxfId="22" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="21" priority="1" operator="greaterThan">
       <formula>10000</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1958,10 +2078,10 @@
     <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Data Entry" error="Please do not input any text or leave any cells blank. If the value is zero, please input zero." promptTitle="Number of Male Employees" prompt="Please input the total number of Male employees in this race/ethnicity and job category" sqref="Q7:Q16">
       <formula1>ISNUMBER(Q7)=TRUE</formula1>
     </dataValidation>
-    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Data Entry" error="Please do not input any text or leave any cells blank. If the value is zero, please input zero." promptTitle="Number of Male Employees" prompt="Please input the total number of male employees in this race/ethnicity and job category" sqref="M7:M16 K7:K16 I7:I16 G7:G16 E7:E16 C7:C16 O7:O16">
+    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Data Entry" error="Please do not input any text or leave any cells blank. If the value is zero, please input zero." promptTitle="Number of Male Employees" prompt="Please input the total number of male employees in this race/ethnicity and job category" sqref="I7:I16 G7:G16 E7:E16 C7:C16 O7:O16 M7:M16 K7:K16">
       <formula1>ISNUMBER(C7)=TRUE</formula1>
     </dataValidation>
-    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Data Entry" error="Please do not input any text or leave any cells blank. If the value is zero, please input zero." promptTitle="Number of Female Employees" prompt="Please input the total number of female employees in this race/ethnicity and job category" sqref="N7:N16 L7:L16 J7:J16 H7:H16 F7:F16 D7:D16 B7:B16 P7:P16">
+    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Data Entry" error="Please do not input any text or leave any cells blank. If the value is zero, please input zero." promptTitle="Number of Female Employees" prompt="Please input the total number of female employees in this race/ethnicity and job category" sqref="J7:J16 H7:H16 F7:F16 D7:D16 B7:B16 P7:P16 N7:N16 L7:L16">
       <formula1>ISNUMBER(B7)=TRUE</formula1>
     </dataValidation>
   </dataValidations>
@@ -1978,7 +2098,7 @@
   </sheetPr>
   <dimension ref="A1:Z17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="92" workbookViewId="0">
+    <sheetView zoomScale="92" workbookViewId="0">
       <selection activeCell="B6" sqref="B6:Q15"/>
     </sheetView>
   </sheetViews>
@@ -2752,10 +2872,10 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Data Entry" error="Please do not input any text or leave any cells blank. If the value is zero, please input zero." promptTitle="Number of Female Employees" prompt="Please input the total number of female employees in this race/ethnicity and job category" sqref="N6:N15 L6:L15 J6:J15 H6:H15 F6:F15 D6:D15 B6:B15 P6:P15">
+    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Data Entry" error="Please do not input any text or leave any cells blank. If the value is zero, please input zero." promptTitle="Number of Female Employees" prompt="Please input the total number of female employees in this race/ethnicity and job category" sqref="J6:J15 H6:H15 F6:F15 D6:D15 B6:B15 P6:P15 N6:N15 L6:L15">
       <formula1>ISNUMBER(B6)=TRUE</formula1>
     </dataValidation>
-    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Data Entry" error="Please do not input any text or leave any cells blank. If the value is zero, please input zero." promptTitle="Number of Male Employees" prompt="Please input the total number of male employees in this race/ethnicity and job category" sqref="M6:M15 K6:K15 I6:I15 G6:G15 E6:E15 C6:C15 O6:O15">
+    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Data Entry" error="Please do not input any text or leave any cells blank. If the value is zero, please input zero." promptTitle="Number of Male Employees" prompt="Please input the total number of male employees in this race/ethnicity and job category" sqref="I6:I15 G6:G15 E6:E15 C6:C15 O6:O15 M6:M15 K6:K15">
       <formula1>ISNUMBER(C6)=TRUE</formula1>
     </dataValidation>
     <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Data Entry" error="Please do not input any text or leave any cells blank. If the value is zero, please input zero." promptTitle="Number of Male Employees" prompt="Please input the total number of Male employees in this race/ethnicity and job category" sqref="Q6:Q15">
@@ -3549,10 +3669,10 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Data Entry" error="Please do not input any text or leave any cells blank. If the value is zero, please input zero." promptTitle="Number of Female Employees" prompt="Please input the total number of female employees in this race/ethnicity and job category" sqref="N6:N15 L6:L15 J6:J15 H6:H15 F6:F15 D6:D15 B6:B15 P6:P15">
+    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Data Entry" error="Please do not input any text or leave any cells blank. If the value is zero, please input zero." promptTitle="Number of Female Employees" prompt="Please input the total number of female employees in this race/ethnicity and job category" sqref="J6:J15 H6:H15 F6:F15 D6:D15 B6:B15 P6:P15 N6:N15 L6:L15">
       <formula1>ISNUMBER(B6)=TRUE</formula1>
     </dataValidation>
-    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Data Entry" error="Please do not input any text or leave any cells blank. If the value is zero, please input zero." promptTitle="Number of Male Employees" prompt="Please input the total number of male employees in this race/ethnicity and job category" sqref="M6:M15 K6:K15 I6:I15 G6:G15 E6:E15 C6:C15 O6:O15">
+    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Data Entry" error="Please do not input any text or leave any cells blank. If the value is zero, please input zero." promptTitle="Number of Male Employees" prompt="Please input the total number of male employees in this race/ethnicity and job category" sqref="I6:I15 G6:G15 E6:E15 C6:C15 O6:O15 M6:M15 K6:K15">
       <formula1>ISNUMBER(C6)=TRUE</formula1>
     </dataValidation>
     <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Data Entry" error="Please do not input any text or leave any cells blank. If the value is zero, please input zero." promptTitle="Number of Male Employees" prompt="Please input the total number of Male employees in this race/ethnicity and job category" sqref="Q6:Q15">
@@ -4346,10 +4466,10 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Data Entry" error="Please do not input any text or leave any cells blank. If the value is zero, please input zero." promptTitle="Number of Female Employees" prompt="Please input the total number of female employees in this race/ethnicity and job category" sqref="N6:N15 L6:L15 J6:J15 H6:H15 F6:F15 D6:D15 B6:B15 P6:P15">
+    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Data Entry" error="Please do not input any text or leave any cells blank. If the value is zero, please input zero." promptTitle="Number of Female Employees" prompt="Please input the total number of female employees in this race/ethnicity and job category" sqref="J6:J15 H6:H15 F6:F15 D6:D15 B6:B15 P6:P15 N6:N15 L6:L15">
       <formula1>ISNUMBER(B6)=TRUE</formula1>
     </dataValidation>
-    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Data Entry" error="Please do not input any text or leave any cells blank. If the value is zero, please input zero." promptTitle="Number of Male Employees" prompt="Please input the total number of male employees in this race/ethnicity and job category" sqref="M6:M15 K6:K15 I6:I15 G6:G15 E6:E15 C6:C15 O6:O15">
+    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Data Entry" error="Please do not input any text or leave any cells blank. If the value is zero, please input zero." promptTitle="Number of Male Employees" prompt="Please input the total number of male employees in this race/ethnicity and job category" sqref="I6:I15 G6:G15 E6:E15 C6:C15 O6:O15 M6:M15 K6:K15">
       <formula1>ISNUMBER(C6)=TRUE</formula1>
     </dataValidation>
     <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Data Entry" error="Please do not input any text or leave any cells blank. If the value is zero, please input zero." promptTitle="Number of Male Employees" prompt="Please input the total number of Male employees in this race/ethnicity and job category" sqref="Q6:Q15">
@@ -5436,16 +5556,16 @@
     <mergeCell ref="J5:K5"/>
   </mergeCells>
   <conditionalFormatting sqref="B7:Q16">
-    <cfRule type="containsText" dxfId="18" priority="1" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="30" priority="1" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",B7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="2" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="29" priority="2" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",B7)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="3" operator="equal">
       <formula>"""Fail"""</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="27" priority="5" operator="greaterThan">
       <formula>10000</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
changed value of cells in sample file
</commit_message>
<xml_diff>
--- a/test/selenium/files/bwwc.xlsx
+++ b/test/selenium/files/bwwc.xlsx
@@ -5,11 +5,11 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lucyqin/Documents/multiparty/web-mpc/test/cafe/files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lucyqin/Documents/multiparty/web-mpc/test/selenium/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16520" activeTab="2"/>
+    <workbookView xWindow="6280" yWindow="1000" windowWidth="28800" windowHeight="16520" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Enter Data →" sheetId="19" r:id="rId1"/>
@@ -631,47 +631,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="23">
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="19">
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -1158,8 +1118,8 @@
   </sheetPr>
   <dimension ref="A1:Z18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S14" sqref="S14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1378,52 +1338,52 @@
         <v>7</v>
       </c>
       <c r="B7" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C7" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D7" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E7" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F7" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G7" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H7" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I7" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J7" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K7" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L7" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M7" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N7" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O7" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P7" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q7" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R7" s="4"/>
       <c r="S7" s="4"/>
@@ -1433,52 +1393,52 @@
         <v>8</v>
       </c>
       <c r="B8" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C8" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D8" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E8" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F8" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G8" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H8" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I8" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J8" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K8" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L8" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M8" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N8" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O8" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P8" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q8" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R8" s="4"/>
       <c r="S8" s="4"/>
@@ -1488,52 +1448,52 @@
         <v>9</v>
       </c>
       <c r="B9" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C9" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D9" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E9" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F9" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G9" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H9" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I9" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J9" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K9" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L9" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M9" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N9" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O9" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P9" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q9" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R9" s="4"/>
       <c r="S9" s="4"/>
@@ -1543,52 +1503,52 @@
         <v>10</v>
       </c>
       <c r="B10" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C10" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D10" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E10" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F10" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G10" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H10" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I10" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J10" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K10" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L10" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M10" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N10" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O10" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P10" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q10" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R10" s="4"/>
       <c r="S10" s="4"/>
@@ -1598,52 +1558,52 @@
         <v>11</v>
       </c>
       <c r="B11" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C11" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D11" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E11" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F11" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G11" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H11" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I11" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J11" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K11" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L11" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M11" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N11" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O11" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P11" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q11" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R11" s="4"/>
       <c r="S11" s="4"/>
@@ -1653,52 +1613,52 @@
         <v>12</v>
       </c>
       <c r="B12" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C12" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D12" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E12" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F12" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G12" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H12" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I12" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J12" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K12" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L12" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M12" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N12" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O12" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P12" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q12" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R12" s="4"/>
       <c r="S12" s="4"/>
@@ -1708,52 +1668,52 @@
         <v>13</v>
       </c>
       <c r="B13" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C13" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D13" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E13" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F13" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G13" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H13" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I13" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J13" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K13" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L13" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M13" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N13" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O13" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P13" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q13" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R13" s="4"/>
       <c r="S13" s="4"/>
@@ -1763,52 +1723,52 @@
         <v>14</v>
       </c>
       <c r="B14" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C14" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D14" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E14" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F14" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G14" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H14" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I14" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J14" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K14" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L14" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M14" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N14" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O14" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P14" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q14" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.2">
@@ -1816,52 +1776,52 @@
         <v>15</v>
       </c>
       <c r="B15" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C15" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D15" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E15" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F15" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G15" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H15" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I15" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J15" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K15" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L15" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M15" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N15" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O15" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P15" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q15" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -1869,52 +1829,52 @@
         <v>16</v>
       </c>
       <c r="B16" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C16" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D16" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E16" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F16" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G16" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H16" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I16" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J16" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K16" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L16" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M16" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N16" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O16" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P16" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q16" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
@@ -1950,7 +1910,7 @@
     <mergeCell ref="J5:K5"/>
   </mergeCells>
   <conditionalFormatting sqref="B7:Q16">
-    <cfRule type="cellIs" dxfId="22" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="greaterThan">
       <formula>10000</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1958,10 +1918,10 @@
     <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Data Entry" error="Please do not input any text or leave any cells blank. If the value is zero, please input zero." promptTitle="Number of Male Employees" prompt="Please input the total number of Male employees in this race/ethnicity and job category" sqref="Q7:Q16">
       <formula1>ISNUMBER(Q7)=TRUE</formula1>
     </dataValidation>
-    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Data Entry" error="Please do not input any text or leave any cells blank. If the value is zero, please input zero." promptTitle="Number of Male Employees" prompt="Please input the total number of male employees in this race/ethnicity and job category" sqref="M7:M16 K7:K16 I7:I16 G7:G16 E7:E16 C7:C16 O7:O16">
+    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Data Entry" error="Please do not input any text or leave any cells blank. If the value is zero, please input zero." promptTitle="Number of Male Employees" prompt="Please input the total number of male employees in this race/ethnicity and job category" sqref="K7:K16 I7:I16 G7:G16 E7:E16 C7:C16 O7:O16 M7:M16">
       <formula1>ISNUMBER(C7)=TRUE</formula1>
     </dataValidation>
-    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Data Entry" error="Please do not input any text or leave any cells blank. If the value is zero, please input zero." promptTitle="Number of Female Employees" prompt="Please input the total number of female employees in this race/ethnicity and job category" sqref="N7:N16 L7:L16 J7:J16 H7:H16 F7:F16 D7:D16 B7:B16 P7:P16">
+    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Data Entry" error="Please do not input any text or leave any cells blank. If the value is zero, please input zero." promptTitle="Number of Female Employees" prompt="Please input the total number of female employees in this race/ethnicity and job category" sqref="L7:L16 J7:J16 H7:H16 F7:F16 D7:D16 B7:B16 P7:P16 N7:N16">
       <formula1>ISNUMBER(B7)=TRUE</formula1>
     </dataValidation>
   </dataValidations>
@@ -1978,7 +1938,7 @@
   </sheetPr>
   <dimension ref="A1:Z17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="92" workbookViewId="0">
+    <sheetView zoomScale="92" workbookViewId="0">
       <selection activeCell="B6" sqref="B6:Q15"/>
     </sheetView>
   </sheetViews>
@@ -2175,52 +2135,52 @@
         <v>7</v>
       </c>
       <c r="B6" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C6" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D6" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E6" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F6" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G6" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H6" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I6" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J6" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K6" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L6" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M6" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N6" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O6" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P6" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q6" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R6" s="4"/>
       <c r="S6" s="4"/>
@@ -2230,52 +2190,52 @@
         <v>8</v>
       </c>
       <c r="B7" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C7" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D7" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E7" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F7" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G7" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H7" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I7" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J7" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K7" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L7" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M7" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N7" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O7" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P7" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q7" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R7" s="4"/>
       <c r="S7" s="4"/>
@@ -2285,52 +2245,52 @@
         <v>9</v>
       </c>
       <c r="B8" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C8" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D8" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E8" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F8" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G8" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H8" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I8" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J8" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K8" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L8" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M8" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N8" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O8" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P8" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q8" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R8" s="4"/>
       <c r="S8" s="4"/>
@@ -2340,52 +2300,52 @@
         <v>10</v>
       </c>
       <c r="B9" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C9" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D9" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E9" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F9" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G9" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H9" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I9" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J9" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K9" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L9" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M9" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N9" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O9" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P9" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q9" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R9" s="4"/>
       <c r="S9" s="4"/>
@@ -2395,52 +2355,52 @@
         <v>11</v>
       </c>
       <c r="B10" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C10" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D10" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E10" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F10" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G10" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H10" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I10" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J10" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K10" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L10" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M10" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N10" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O10" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P10" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q10" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R10" s="4"/>
       <c r="S10" s="4"/>
@@ -2450,52 +2410,52 @@
         <v>12</v>
       </c>
       <c r="B11" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C11" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D11" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E11" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F11" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G11" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H11" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I11" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J11" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K11" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L11" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M11" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N11" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O11" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P11" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q11" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R11" s="4"/>
       <c r="S11" s="4"/>
@@ -2505,52 +2465,52 @@
         <v>13</v>
       </c>
       <c r="B12" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C12" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D12" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E12" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F12" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G12" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H12" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I12" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J12" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K12" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L12" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M12" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N12" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O12" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P12" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q12" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R12" s="4"/>
       <c r="S12" s="4"/>
@@ -2560,52 +2520,52 @@
         <v>14</v>
       </c>
       <c r="B13" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C13" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D13" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E13" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F13" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G13" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H13" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I13" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J13" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K13" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L13" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M13" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N13" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O13" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P13" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q13" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.2">
@@ -2613,52 +2573,52 @@
         <v>15</v>
       </c>
       <c r="B14" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C14" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D14" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E14" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F14" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G14" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H14" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I14" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J14" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K14" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L14" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M14" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N14" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O14" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P14" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q14" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -2666,52 +2626,52 @@
         <v>16</v>
       </c>
       <c r="B15" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C15" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D15" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E15" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F15" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G15" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H15" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I15" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J15" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K15" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L15" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M15" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N15" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O15" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P15" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q15" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.2">
@@ -2747,15 +2707,15 @@
     <mergeCell ref="J4:K4"/>
   </mergeCells>
   <conditionalFormatting sqref="B6:Q15">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="17" priority="1" operator="greaterThan">
       <formula>10000</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Data Entry" error="Please do not input any text or leave any cells blank. If the value is zero, please input zero." promptTitle="Number of Female Employees" prompt="Please input the total number of female employees in this race/ethnicity and job category" sqref="N6:N15 L6:L15 J6:J15 H6:H15 F6:F15 D6:D15 B6:B15 P6:P15">
+    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Data Entry" error="Please do not input any text or leave any cells blank. If the value is zero, please input zero." promptTitle="Number of Female Employees" prompt="Please input the total number of female employees in this race/ethnicity and job category" sqref="L6:L15 J6:J15 H6:H15 F6:F15 D6:D15 B6:B15 P6:P15 N6:N15">
       <formula1>ISNUMBER(B6)=TRUE</formula1>
     </dataValidation>
-    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Data Entry" error="Please do not input any text or leave any cells blank. If the value is zero, please input zero." promptTitle="Number of Male Employees" prompt="Please input the total number of male employees in this race/ethnicity and job category" sqref="M6:M15 K6:K15 I6:I15 G6:G15 E6:E15 C6:C15 O6:O15">
+    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Data Entry" error="Please do not input any text or leave any cells blank. If the value is zero, please input zero." promptTitle="Number of Male Employees" prompt="Please input the total number of male employees in this race/ethnicity and job category" sqref="K6:K15 I6:I15 G6:G15 E6:E15 C6:C15 O6:O15 M6:M15">
       <formula1>ISNUMBER(C6)=TRUE</formula1>
     </dataValidation>
     <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Data Entry" error="Please do not input any text or leave any cells blank. If the value is zero, please input zero." promptTitle="Number of Male Employees" prompt="Please input the total number of Male employees in this race/ethnicity and job category" sqref="Q6:Q15">
@@ -2972,52 +2932,52 @@
         <v>7</v>
       </c>
       <c r="B6" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C6" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D6" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E6" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F6" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G6" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H6" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I6" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J6" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K6" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L6" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M6" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N6" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O6" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P6" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q6" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R6" s="4"/>
       <c r="S6" s="4"/>
@@ -3027,52 +2987,52 @@
         <v>8</v>
       </c>
       <c r="B7" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C7" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D7" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E7" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F7" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G7" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H7" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I7" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J7" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K7" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L7" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M7" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N7" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O7" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P7" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q7" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R7" s="4"/>
       <c r="S7" s="4"/>
@@ -3082,52 +3042,52 @@
         <v>9</v>
       </c>
       <c r="B8" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C8" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D8" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E8" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F8" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G8" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H8" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I8" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J8" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K8" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L8" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M8" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N8" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O8" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P8" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q8" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R8" s="4"/>
       <c r="S8" s="4"/>
@@ -3137,52 +3097,52 @@
         <v>10</v>
       </c>
       <c r="B9" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C9" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D9" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E9" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F9" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G9" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H9" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I9" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J9" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K9" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L9" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M9" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N9" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O9" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P9" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q9" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R9" s="4"/>
       <c r="S9" s="4"/>
@@ -3192,52 +3152,52 @@
         <v>11</v>
       </c>
       <c r="B10" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C10" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D10" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E10" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F10" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G10" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H10" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I10" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J10" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K10" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L10" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M10" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N10" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O10" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P10" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q10" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R10" s="4"/>
       <c r="S10" s="4"/>
@@ -3247,52 +3207,52 @@
         <v>12</v>
       </c>
       <c r="B11" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C11" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D11" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E11" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F11" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G11" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H11" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I11" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J11" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K11" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L11" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M11" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N11" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O11" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P11" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q11" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R11" s="4"/>
       <c r="S11" s="4"/>
@@ -3302,52 +3262,52 @@
         <v>13</v>
       </c>
       <c r="B12" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C12" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D12" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E12" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F12" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G12" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H12" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I12" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J12" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K12" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L12" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M12" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N12" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O12" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P12" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q12" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R12" s="4"/>
       <c r="S12" s="4"/>
@@ -3357,52 +3317,52 @@
         <v>14</v>
       </c>
       <c r="B13" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C13" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D13" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E13" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F13" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G13" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H13" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I13" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J13" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K13" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L13" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M13" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N13" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O13" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P13" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q13" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.2">
@@ -3410,52 +3370,52 @@
         <v>15</v>
       </c>
       <c r="B14" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C14" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D14" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E14" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F14" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G14" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H14" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I14" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J14" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K14" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L14" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M14" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N14" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O14" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P14" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q14" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -3463,52 +3423,52 @@
         <v>16</v>
       </c>
       <c r="B15" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C15" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D15" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E15" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F15" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G15" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H15" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I15" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J15" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K15" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L15" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M15" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N15" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O15" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P15" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q15" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.2">
@@ -3549,10 +3509,10 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Data Entry" error="Please do not input any text or leave any cells blank. If the value is zero, please input zero." promptTitle="Number of Female Employees" prompt="Please input the total number of female employees in this race/ethnicity and job category" sqref="N6:N15 L6:L15 J6:J15 H6:H15 F6:F15 D6:D15 B6:B15 P6:P15">
+    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Data Entry" error="Please do not input any text or leave any cells blank. If the value is zero, please input zero." promptTitle="Number of Female Employees" prompt="Please input the total number of female employees in this race/ethnicity and job category" sqref="L6:L15 J6:J15 H6:H15 F6:F15 D6:D15 B6:B15 P6:P15 N6:N15">
       <formula1>ISNUMBER(B6)=TRUE</formula1>
     </dataValidation>
-    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Data Entry" error="Please do not input any text or leave any cells blank. If the value is zero, please input zero." promptTitle="Number of Male Employees" prompt="Please input the total number of male employees in this race/ethnicity and job category" sqref="M6:M15 K6:K15 I6:I15 G6:G15 E6:E15 C6:C15 O6:O15">
+    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Data Entry" error="Please do not input any text or leave any cells blank. If the value is zero, please input zero." promptTitle="Number of Male Employees" prompt="Please input the total number of male employees in this race/ethnicity and job category" sqref="K6:K15 I6:I15 G6:G15 E6:E15 C6:C15 O6:O15 M6:M15">
       <formula1>ISNUMBER(C6)=TRUE</formula1>
     </dataValidation>
     <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Data Entry" error="Please do not input any text or leave any cells blank. If the value is zero, please input zero." promptTitle="Number of Male Employees" prompt="Please input the total number of Male employees in this race/ethnicity and job category" sqref="Q6:Q15">
@@ -3769,52 +3729,52 @@
         <v>7</v>
       </c>
       <c r="B6" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C6" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D6" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E6" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F6" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G6" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H6" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I6" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J6" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K6" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L6" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M6" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N6" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O6" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P6" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q6" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R6" s="4"/>
       <c r="S6" s="4"/>
@@ -3824,52 +3784,52 @@
         <v>8</v>
       </c>
       <c r="B7" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C7" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D7" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E7" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F7" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G7" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H7" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I7" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J7" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K7" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L7" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M7" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N7" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O7" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P7" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q7" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R7" s="4"/>
       <c r="S7" s="4"/>
@@ -3879,52 +3839,52 @@
         <v>9</v>
       </c>
       <c r="B8" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C8" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D8" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E8" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F8" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G8" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H8" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I8" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J8" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K8" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L8" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M8" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N8" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O8" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P8" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q8" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R8" s="4"/>
       <c r="S8" s="4"/>
@@ -3934,52 +3894,52 @@
         <v>10</v>
       </c>
       <c r="B9" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C9" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D9" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E9" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F9" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G9" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H9" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I9" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J9" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K9" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L9" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M9" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N9" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O9" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P9" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q9" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R9" s="4"/>
       <c r="S9" s="4"/>
@@ -3989,52 +3949,52 @@
         <v>11</v>
       </c>
       <c r="B10" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C10" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D10" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E10" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F10" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G10" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H10" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I10" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J10" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K10" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L10" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M10" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N10" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O10" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P10" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q10" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R10" s="4"/>
       <c r="S10" s="4"/>
@@ -4044,52 +4004,52 @@
         <v>12</v>
       </c>
       <c r="B11" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C11" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D11" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E11" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F11" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G11" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H11" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I11" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J11" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K11" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L11" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M11" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N11" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O11" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P11" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q11" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R11" s="4"/>
       <c r="S11" s="4"/>
@@ -4099,52 +4059,52 @@
         <v>13</v>
       </c>
       <c r="B12" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C12" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D12" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E12" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F12" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G12" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H12" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I12" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J12" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K12" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L12" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M12" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N12" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O12" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P12" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q12" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R12" s="4"/>
       <c r="S12" s="4"/>
@@ -4154,52 +4114,52 @@
         <v>14</v>
       </c>
       <c r="B13" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C13" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D13" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E13" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F13" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G13" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H13" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I13" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J13" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K13" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L13" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M13" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N13" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O13" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P13" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q13" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.2">
@@ -4207,52 +4167,52 @@
         <v>15</v>
       </c>
       <c r="B14" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C14" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D14" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E14" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F14" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G14" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H14" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I14" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J14" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K14" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L14" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M14" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N14" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O14" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P14" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q14" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -4260,52 +4220,52 @@
         <v>16</v>
       </c>
       <c r="B15" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C15" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D15" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E15" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F15" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G15" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H15" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I15" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J15" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K15" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L15" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M15" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N15" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O15" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P15" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q15" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.2">
@@ -4346,10 +4306,10 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Data Entry" error="Please do not input any text or leave any cells blank. If the value is zero, please input zero." promptTitle="Number of Female Employees" prompt="Please input the total number of female employees in this race/ethnicity and job category" sqref="N6:N15 L6:L15 J6:J15 H6:H15 F6:F15 D6:D15 B6:B15 P6:P15">
+    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Data Entry" error="Please do not input any text or leave any cells blank. If the value is zero, please input zero." promptTitle="Number of Female Employees" prompt="Please input the total number of female employees in this race/ethnicity and job category" sqref="L6:L15 J6:J15 H6:H15 F6:F15 D6:D15 B6:B15 P6:P15 N6:N15">
       <formula1>ISNUMBER(B6)=TRUE</formula1>
     </dataValidation>
-    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Data Entry" error="Please do not input any text or leave any cells blank. If the value is zero, please input zero." promptTitle="Number of Male Employees" prompt="Please input the total number of male employees in this race/ethnicity and job category" sqref="M6:M15 K6:K15 I6:I15 G6:G15 E6:E15 C6:C15 O6:O15">
+    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Data Entry" error="Please do not input any text or leave any cells blank. If the value is zero, please input zero." promptTitle="Number of Male Employees" prompt="Please input the total number of male employees in this race/ethnicity and job category" sqref="K6:K15 I6:I15 G6:G15 E6:E15 C6:C15 O6:O15 M6:M15">
       <formula1>ISNUMBER(C6)=TRUE</formula1>
     </dataValidation>
     <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Data Entry" error="Please do not input any text or leave any cells blank. If the value is zero, please input zero." promptTitle="Number of Male Employees" prompt="Please input the total number of Male employees in this race/ethnicity and job category" sqref="Q6:Q15">
@@ -4434,15 +4394,15 @@
       </c>
       <c r="B6" s="27">
         <f t="array" ref="B6">SUM((B$5='1.Number of Employees'!$B$6:$Q$6)*('1.Number of Employees'!$B$7:$Q$16))</f>
-        <v>80</v>
+        <v>160</v>
       </c>
       <c r="C6" s="27">
         <f t="array" ref="C6">SUM((C$5='1.Number of Employees'!$B$6:$Q$6)*('1.Number of Employees'!$B$7:$Q$16))</f>
-        <v>80</v>
+        <v>160</v>
       </c>
       <c r="D6" s="28">
         <f>SUM($B$6:$C$6)</f>
-        <v>160</v>
+        <v>320</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -5436,16 +5396,16 @@
     <mergeCell ref="J5:K5"/>
   </mergeCells>
   <conditionalFormatting sqref="B7:Q16">
-    <cfRule type="containsText" dxfId="18" priority="1" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="14" priority="1" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",B7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="2" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="13" priority="2" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",B7)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="3" operator="equal">
       <formula>"""Fail"""</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="11" priority="5" operator="greaterThan">
       <formula>10000</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>